<commit_message>
added changes in the weekly report excel genartion module
</commit_message>
<xml_diff>
--- a/week_report_cal.xlsx
+++ b/week_report_cal.xlsx
@@ -201,8 +201,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -211,7 +209,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -220,51 +226,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6096000" y="190500"/>
-          <a:ext cx="1304925" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -555,7 +516,7 @@
   <dimension ref="A2:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -575,65 +536,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="9" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="1" t="s">
+      <c r="H5" s="2"/>
+      <c r="I5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="9" t="s">
+      <c r="J5" s="2"/>
+      <c r="K5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="2" t="s">
+      <c r="L5" s="2"/>
+      <c r="M5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="7"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="K2:M3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>